<commit_message>
Resolving merge conflict by merging main into branch before remerging to master
</commit_message>
<xml_diff>
--- a/CoilDesign/AnalysisResult_LessFerrites/Less Ferrites.xlsx
+++ b/CoilDesign/AnalysisResult_LessFerrites/Less Ferrites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\files.auckland.ac.nz\myhome\Documents\GitHub\2020-srw-rc-car\CoilDesign\AnalysisResult_LessFerrites\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2587969-7183-423C-82BD-67275FB58225}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDA4F80-0AF3-4109-8849-AC663CB1F9CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,19 +28,12 @@
     <definedName name="w" localSheetId="0">ydisp!$K$2</definedName>
     <definedName name="w">xdisp!$K$2</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="376">
   <si>
     <t>Variation</t>
   </si>
@@ -1147,6 +1140,27 @@
   </si>
   <si>
     <t>7 Ferrites Y sweep (in Gap)</t>
+  </si>
+  <si>
+    <t>Lpt_new ()</t>
+  </si>
+  <si>
+    <t>L_st ()</t>
+  </si>
+  <si>
+    <t>k_nominal ()</t>
+  </si>
+  <si>
+    <t>Mpt_st ()</t>
+  </si>
+  <si>
+    <t>7 Ferrites Y sweep (in Gap,   SINGLE instead of double ferrites side-by-side)</t>
+  </si>
+  <si>
+    <t>7 Ferrites y sweep (SINGLE on Top)</t>
+  </si>
+  <si>
+    <t>min 8 ferrites</t>
   </si>
 </sst>
 </file>
@@ -5796,10 +5810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D02989-F4B6-4C9B-BB89-45B9B948CA00}">
-  <dimension ref="B1:AA119"/>
+  <dimension ref="B1:AA137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="H111" sqref="H111"/>
+    <sheetView tabSelected="1" topLeftCell="G80" workbookViewId="0">
+      <selection activeCell="V116" sqref="V116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5871,16 +5885,16 @@
         <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>369</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
+        <v>370</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>329</v>
+        <v>371</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>372</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>18</v>
@@ -6124,7 +6138,7 @@
         <v>12.377922385027425</v>
       </c>
       <c r="V7" s="5">
-        <f t="shared" si="18"/>
+        <f>U7*$N$1</f>
         <v>61.889611925137125</v>
       </c>
       <c r="W7" s="4"/>
@@ -11709,16 +11723,16 @@
         <v>13</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>15</v>
+        <v>369</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>14</v>
+        <v>370</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>329</v>
+        <v>371</v>
       </c>
       <c r="G80" t="s">
-        <v>16</v>
+        <v>372</v>
       </c>
       <c r="H80" s="1" t="s">
         <v>18</v>
@@ -13515,24 +13529,9 @@
       <c r="Y107" s="4"/>
     </row>
     <row r="108" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B108" t="s">
-        <v>0</v>
-      </c>
-      <c r="C108" t="s">
-        <v>2</v>
-      </c>
-      <c r="D108" t="s">
-        <v>3</v>
-      </c>
-      <c r="E108" t="s">
-        <v>4</v>
-      </c>
-      <c r="F108" t="s">
-        <v>5</v>
-      </c>
-      <c r="G108" t="s">
-        <v>6</v>
-      </c>
+      <c r="D108"/>
+      <c r="E108"/>
+      <c r="G108"/>
       <c r="J108" s="2"/>
       <c r="S108" s="4"/>
       <c r="T108" s="4"/>
@@ -13543,104 +13542,98 @@
       <c r="Y108" s="4"/>
     </row>
     <row r="109" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B109">
-        <v>1</v>
-      </c>
       <c r="C109">
         <v>0</v>
       </c>
       <c r="D109">
-        <v>2673.0484385991199</v>
+        <v>2426.7780120000002</v>
       </c>
       <c r="E109">
-        <v>142.88278312456899</v>
+        <v>126.0292267</v>
       </c>
       <c r="F109">
-        <v>0.14988581070243401</v>
+        <v>9.0622852000000004E-2</v>
       </c>
       <c r="G109">
-        <v>92.630473943514104</v>
+        <v>50.117383490000002</v>
       </c>
       <c r="H109" s="1">
-        <f t="shared" ref="H106:H119" si="78">2*PI()*150000*Ipt*Ipt*D109*(10^-9)</f>
-        <v>62.982220030444964</v>
+        <f t="shared" ref="H109:H114" si="78">2*PI()*150000*Ipt*Ipt*D109*(10^-9)</f>
+        <v>57.179609807943322</v>
       </c>
       <c r="I109" s="1">
-        <f t="shared" ref="I106:I119" si="79">2*PI()*150000*Ist*Ist*E109*(10^-9)</f>
+        <f t="shared" ref="I109:I114" si="79">2*PI()*150000*Ist*Ist*E109*(10^-9)</f>
         <v>0</v>
       </c>
       <c r="J109" s="2">
-        <f t="shared" ref="J106:J119" si="80">F109*SQRT(H109*I109)</f>
+        <f t="shared" ref="J109:J114" si="80">F109*SQRT(H109*I109)</f>
         <v>0</v>
       </c>
       <c r="K109">
-        <f t="shared" ref="K106:K119" si="81">2*PI()*150000*G109*Ipt*(10^-9)</f>
-        <v>0.43651082465922703</v>
+        <f t="shared" ref="K109:K114" si="81">2*PI()*150000*G109*Ipt*(10^-9)</f>
+        <v>0.23617260568398959</v>
       </c>
       <c r="N109">
-        <f t="shared" ref="N106:N119" si="82">D109*$D$1^2*10^-3</f>
-        <v>24.057435947392079</v>
+        <f t="shared" ref="N109:N114" si="82">D109*$D$1^2*10^-3</f>
+        <v>21.841002108000001</v>
       </c>
       <c r="O109">
-        <f t="shared" ref="O106:O119" si="83">E109*$D$2^2*10^-3</f>
-        <v>3.5720695781142249</v>
+        <f t="shared" ref="O109:O114" si="83">E109*$D$2^2*10^-3</f>
+        <v>3.1507306675</v>
       </c>
       <c r="P109">
-        <f t="shared" ref="P106:P119" si="84">G109*$D$1*$D$2*10^-3</f>
-        <v>1.3894571091527115</v>
+        <f t="shared" ref="P109:P114" si="84">G109*$D$1*$D$2*10^-3</f>
+        <v>0.75176075234999995</v>
       </c>
       <c r="Q109">
-        <f t="shared" ref="Q106:Q119" si="85">P109/SQRT(N109*O109)</f>
-        <v>0.14988581070243362</v>
+        <f t="shared" ref="Q109:Q114" si="85">P109/SQRT(N109*O109)</f>
+        <v>9.0622852466814341E-2</v>
       </c>
       <c r="S109" s="4">
-        <f t="shared" ref="S106:S119" si="86">w*P109*10^-6*$G$1</f>
-        <v>6.5476623698884042</v>
+        <f t="shared" ref="S109:S114" si="86">w*P109*10^-6*$G$1</f>
+        <v>3.5425890852598432</v>
       </c>
       <c r="T109" s="4">
-        <f t="shared" ref="T106:T119" si="87">P109*$G$1/O109</f>
-        <v>1.9448908801578229</v>
+        <f t="shared" ref="T109:T114" si="87">P109*$G$1/O109</f>
+        <v>1.1929943109775505</v>
       </c>
       <c r="U109" s="4">
-        <f t="shared" ref="U106:U119" si="88">S109*T109</f>
-        <v>12.734488829548514</v>
+        <f t="shared" ref="U109:U114" si="88">S109*T109</f>
+        <v>4.2262886248461573</v>
       </c>
       <c r="V109" s="5">
-        <f t="shared" ref="V106:V119" si="89">U109*$N$1</f>
-        <v>63.672444147742567</v>
+        <f t="shared" ref="V109:V114" si="89">U109*$N$1</f>
+        <v>21.131443124230785</v>
       </c>
       <c r="W109" s="4"/>
       <c r="X109" s="4">
-        <f t="shared" ref="X106:X119" si="90">w*N109*10^-6*$G$1</f>
-        <v>113.36799605480094</v>
+        <f t="shared" ref="X109:X114" si="90">w*N109*10^-6*$G$1</f>
+        <v>102.92329765429798</v>
       </c>
       <c r="Y109" s="4">
-        <f t="shared" ref="Y106:Y119" si="91">X109*$G$1</f>
-        <v>566.83998027400469</v>
+        <f t="shared" ref="Y109:Y114" si="91">X109*$G$1</f>
+        <v>514.61648827148997</v>
       </c>
     </row>
     <row r="110" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B110">
-        <v>2</v>
-      </c>
       <c r="C110">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D110">
-        <v>2674.08016081305</v>
+        <v>2425.916815</v>
       </c>
       <c r="E110">
-        <v>142.93981539001601</v>
+        <v>125.93062</v>
       </c>
       <c r="F110">
-        <v>0.14917679876224199</v>
+        <v>8.9420795999999997E-2</v>
       </c>
       <c r="G110">
-        <v>92.228490931029597</v>
+        <v>49.42448547</v>
       </c>
       <c r="H110" s="1">
         <f t="shared" si="78"/>
-        <v>63.00652941240368</v>
+        <v>57.159318331679621</v>
       </c>
       <c r="I110" s="1">
         <f t="shared" si="79"/>
@@ -13652,72 +13645,69 @@
       </c>
       <c r="K110">
         <f t="shared" si="81"/>
-        <v>0.43461652434089315</v>
+        <v>0.23290740069001123</v>
       </c>
       <c r="N110">
         <f t="shared" si="82"/>
-        <v>24.066721447317452</v>
+        <v>21.833251335</v>
       </c>
       <c r="O110">
         <f t="shared" si="83"/>
-        <v>3.5734953847504003</v>
+        <v>3.1482654999999999</v>
       </c>
       <c r="P110">
         <f t="shared" si="84"/>
-        <v>1.3834273639654442</v>
+        <v>0.74136728205000002</v>
       </c>
       <c r="Q110">
         <f t="shared" si="85"/>
-        <v>0.14917679876224232</v>
+        <v>8.9420796439828892E-2</v>
       </c>
       <c r="S110" s="4">
         <f t="shared" si="86"/>
-        <v>6.5192478651133978</v>
+        <v>3.4936110103501683</v>
       </c>
       <c r="T110" s="4">
         <f t="shared" si="87"/>
-        <v>1.935678117661922</v>
+        <v>1.177421793127041</v>
       </c>
       <c r="U110" s="4">
         <f t="shared" si="88"/>
-        <v>12.619165436114205</v>
+        <v>4.1134537402948688</v>
       </c>
       <c r="V110" s="5">
         <f t="shared" si="89"/>
-        <v>63.095827180571021</v>
+        <v>20.567268701474344</v>
       </c>
       <c r="W110" s="4"/>
       <c r="X110" s="4">
         <f t="shared" si="90"/>
-        <v>113.41175294232663</v>
+        <v>102.8867729970233</v>
       </c>
       <c r="Y110" s="4">
         <f t="shared" si="91"/>
-        <v>567.0587647116331</v>
+        <v>514.43386498511654</v>
       </c>
     </row>
     <row r="111" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B111">
-        <v>3</v>
-      </c>
       <c r="C111">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D111">
-        <v>2671.3322043072499</v>
+        <v>2421.8383140000001</v>
       </c>
       <c r="E111">
-        <v>143.003695597366</v>
+        <v>125.9062314</v>
       </c>
       <c r="F111">
-        <v>0.14689138345290401</v>
+        <v>8.5622882999999997E-2</v>
       </c>
       <c r="G111">
-        <v>90.789139841327994</v>
+        <v>47.280932440000001</v>
       </c>
       <c r="H111" s="1">
         <f t="shared" si="78"/>
-        <v>62.941782212621135</v>
+        <v>57.063220915835188</v>
       </c>
       <c r="I111" s="1">
         <f t="shared" si="79"/>
@@ -13729,72 +13719,69 @@
       </c>
       <c r="K111">
         <f t="shared" si="81"/>
-        <v>0.42783374212687864</v>
+        <v>0.22280614501256901</v>
       </c>
       <c r="N111">
         <f t="shared" si="82"/>
-        <v>24.04198983876525</v>
+        <v>21.796544826000002</v>
       </c>
       <c r="O111">
         <f t="shared" si="83"/>
-        <v>3.57509238993415</v>
+        <v>3.147655785</v>
       </c>
       <c r="P111">
         <f t="shared" si="84"/>
-        <v>1.3618370976199199</v>
+        <v>0.70921398660000001</v>
       </c>
       <c r="Q111">
         <f t="shared" si="85"/>
-        <v>0.1468913834529039</v>
+        <v>8.5622883145012721E-2</v>
       </c>
       <c r="S111" s="4">
         <f t="shared" si="86"/>
-        <v>6.4175061319031794</v>
+        <v>3.3420921751885349</v>
       </c>
       <c r="T111" s="4">
         <f t="shared" si="87"/>
-        <v>1.9046180477100951</v>
+        <v>1.1265748783264751</v>
       </c>
       <c r="U111" s="4">
         <f t="shared" si="88"/>
-        <v>12.222898000112998</v>
+        <v>3.765117085618888</v>
       </c>
       <c r="V111" s="5">
         <f t="shared" si="89"/>
-        <v>61.114490000564992</v>
+        <v>18.825585428094442</v>
       </c>
       <c r="W111" s="4"/>
       <c r="X111" s="4">
         <f t="shared" si="90"/>
-        <v>113.29520798271804</v>
+        <v>102.71379764850332</v>
       </c>
       <c r="Y111" s="4">
         <f t="shared" si="91"/>
-        <v>566.47603991359017</v>
+        <v>513.56898824251653</v>
       </c>
     </row>
     <row r="112" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B112">
-        <v>4</v>
-      </c>
       <c r="C112">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D112">
-        <v>2669.9693238208001</v>
+        <v>2420.351349</v>
       </c>
       <c r="E112">
-        <v>143.13108532127501</v>
+        <v>125.9120786</v>
       </c>
       <c r="F112">
-        <v>0.14313586624800001</v>
+        <v>7.9452495999999997E-2</v>
       </c>
       <c r="G112">
-        <v>88.484782701693007</v>
+        <v>43.8611942</v>
       </c>
       <c r="H112" s="1">
         <f t="shared" si="78"/>
-        <v>62.909670097691503</v>
+        <v>57.028185128434096</v>
       </c>
       <c r="I112" s="1">
         <f t="shared" si="79"/>
@@ -13806,72 +13793,69 @@
       </c>
       <c r="K112">
         <f t="shared" si="81"/>
-        <v>0.41697471493519195</v>
+        <v>0.20669100821459288</v>
       </c>
       <c r="N112">
         <f t="shared" si="82"/>
-        <v>24.029723914387201</v>
+        <v>21.783162141000002</v>
       </c>
       <c r="O112">
         <f t="shared" si="83"/>
-        <v>3.5782771330318752</v>
+        <v>3.1478019650000002</v>
       </c>
       <c r="P112">
         <f t="shared" si="84"/>
-        <v>1.3272717405253953</v>
+        <v>0.65791791300000002</v>
       </c>
       <c r="Q112">
         <f t="shared" si="85"/>
-        <v>0.14313586624799995</v>
+        <v>7.945249650429935E-2</v>
       </c>
       <c r="S112" s="4">
         <f t="shared" si="86"/>
-        <v>6.2546207240278795</v>
+        <v>3.1003651232188929</v>
       </c>
       <c r="T112" s="4">
         <f t="shared" si="87"/>
-        <v>1.8546240148269311</v>
+        <v>1.045043367269135</v>
       </c>
       <c r="U112" s="4">
         <f t="shared" si="88"/>
-        <v>11.599969798416312</v>
+        <v>3.2400160081324585</v>
       </c>
       <c r="V112" s="5">
         <f t="shared" si="89"/>
-        <v>57.99984899208156</v>
+        <v>16.200080040662293</v>
       </c>
       <c r="W112" s="4"/>
       <c r="X112" s="4">
         <f t="shared" si="90"/>
-        <v>113.23740617584468</v>
+        <v>102.65073323118136</v>
       </c>
       <c r="Y112" s="4">
         <f t="shared" si="91"/>
-        <v>566.18703087922336</v>
+        <v>513.25366615590679</v>
       </c>
     </row>
     <row r="113" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B113">
-        <v>5</v>
-      </c>
       <c r="C113">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D113">
-        <v>2664.71691007864</v>
+        <v>2414.8736410000001</v>
       </c>
       <c r="E113">
-        <v>143.04348326533199</v>
+        <v>125.8301465</v>
       </c>
       <c r="F113">
-        <v>0.13806825899900499</v>
+        <v>7.0770549000000002E-2</v>
       </c>
       <c r="G113">
-        <v>85.241959810665506</v>
+        <v>39.011452669999997</v>
       </c>
       <c r="H113" s="1">
         <f t="shared" si="78"/>
-        <v>62.785913014496614</v>
+        <v>56.899119674349272</v>
       </c>
       <c r="I113" s="1">
         <f t="shared" si="79"/>
@@ -13883,72 +13867,69 @@
       </c>
       <c r="K113">
         <f t="shared" si="81"/>
-        <v>0.40169327207817473</v>
+        <v>0.18383713967090684</v>
       </c>
       <c r="N113">
         <f t="shared" si="82"/>
-        <v>23.982452190707761</v>
+        <v>21.733862768999998</v>
       </c>
       <c r="O113">
         <f t="shared" si="83"/>
-        <v>3.5760870816332995</v>
+        <v>3.1457536624999998</v>
       </c>
       <c r="P113">
         <f t="shared" si="84"/>
-        <v>1.2786293971599825</v>
+        <v>0.58517179004999997</v>
       </c>
       <c r="Q113">
         <f t="shared" si="85"/>
-        <v>0.13806825899900502</v>
+        <v>7.0770549185016865E-2</v>
       </c>
       <c r="S113" s="4">
         <f t="shared" si="86"/>
-        <v>6.0253990811726199</v>
+        <v>2.757557095063603</v>
       </c>
       <c r="T113" s="4">
         <f t="shared" si="87"/>
-        <v>1.7877492465535774</v>
+        <v>0.93009792379125933</v>
       </c>
       <c r="U113" s="4">
         <f t="shared" si="88"/>
-        <v>10.771902667550968</v>
+        <v>2.5647981288545134</v>
       </c>
       <c r="V113" s="5">
         <f t="shared" si="89"/>
-        <v>53.859513337754841</v>
+        <v>12.823990644272566</v>
       </c>
       <c r="W113" s="4"/>
       <c r="X113" s="4">
         <f t="shared" si="90"/>
-        <v>113.01464342609391</v>
+        <v>102.41841541382865</v>
       </c>
       <c r="Y113" s="4">
         <f t="shared" si="91"/>
-        <v>565.07321713046952</v>
+        <v>512.09207706914322</v>
       </c>
     </row>
     <row r="114" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B114">
-        <v>6</v>
-      </c>
       <c r="C114">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="D114">
-        <v>2660.4509343518698</v>
+        <v>2414.540536</v>
       </c>
       <c r="E114">
-        <v>143.22456014361501</v>
+        <v>125.995983</v>
       </c>
       <c r="F114">
-        <v>0.131571743142994</v>
+        <v>5.9807707000000002E-2</v>
       </c>
       <c r="G114">
-        <v>81.217385346062002</v>
+        <v>32.98775449</v>
       </c>
       <c r="H114" s="1">
         <f t="shared" si="78"/>
-        <v>62.685398329469514</v>
+        <v>56.891271072692717</v>
       </c>
       <c r="I114" s="1">
         <f t="shared" si="79"/>
@@ -13960,433 +13941,1164 @@
       </c>
       <c r="K114">
         <f t="shared" si="81"/>
-        <v>0.38272791172043957</v>
+        <v>0.15545113074631159</v>
       </c>
       <c r="N114">
         <f t="shared" si="82"/>
-        <v>23.944058409166828</v>
+        <v>21.730864824000001</v>
       </c>
       <c r="O114">
         <f t="shared" si="83"/>
-        <v>3.5806140035903753</v>
+        <v>3.1498995750000001</v>
       </c>
       <c r="P114">
         <f t="shared" si="84"/>
-        <v>1.21826078019093</v>
+        <v>0.49481631735000003</v>
       </c>
       <c r="Q114">
         <f t="shared" si="85"/>
-        <v>0.13157174314299394</v>
+        <v>5.9807707218594561E-2</v>
       </c>
       <c r="S114" s="4">
         <f t="shared" si="86"/>
-        <v>5.7409186758065935</v>
+        <v>2.3317669611946736</v>
       </c>
       <c r="T114" s="4">
         <f t="shared" si="87"/>
-        <v>1.7011897665726436</v>
+        <v>0.78544776677523132</v>
       </c>
       <c r="U114" s="4">
         <f t="shared" si="88"/>
-        <v>9.7663921020079485</v>
+        <v>1.8314811523106238</v>
       </c>
       <c r="V114" s="5">
         <f t="shared" si="89"/>
-        <v>48.831960510039742</v>
+        <v>9.1574057615531181</v>
       </c>
       <c r="W114" s="4"/>
       <c r="X114" s="4">
         <f t="shared" si="90"/>
-        <v>112.83371699304512</v>
+        <v>102.40428793084688</v>
       </c>
       <c r="Y114" s="4">
         <f t="shared" si="91"/>
-        <v>564.16858496522559</v>
+        <v>512.02143965423443</v>
       </c>
     </row>
     <row r="115" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B115">
-        <v>7</v>
-      </c>
-      <c r="C115">
-        <v>30</v>
-      </c>
-      <c r="D115">
-        <v>2653.3901926952799</v>
-      </c>
-      <c r="E115">
-        <v>143.008857038283</v>
-      </c>
-      <c r="F115">
-        <v>0.123931707256746</v>
-      </c>
-      <c r="G115">
-        <v>76.342162908459599</v>
-      </c>
-      <c r="H115" s="1">
-        <f t="shared" si="78"/>
-        <v>62.519033523590231</v>
-      </c>
-      <c r="I115" s="1">
-        <f t="shared" si="79"/>
-        <v>0</v>
-      </c>
-      <c r="J115" s="2">
-        <f t="shared" si="80"/>
-        <v>0</v>
-      </c>
-      <c r="K115">
-        <f t="shared" si="81"/>
-        <v>0.35975396722855785</v>
-      </c>
-      <c r="N115">
-        <f t="shared" si="82"/>
-        <v>23.880511734257517</v>
-      </c>
-      <c r="O115">
-        <f t="shared" si="83"/>
-        <v>3.5752214259570754</v>
-      </c>
-      <c r="P115">
-        <f t="shared" si="84"/>
-        <v>1.1451324436268939</v>
-      </c>
-      <c r="Q115">
-        <f t="shared" si="85"/>
-        <v>0.12393170725674622</v>
-      </c>
-      <c r="S115" s="4">
-        <f t="shared" si="86"/>
-        <v>5.3963095084283665</v>
-      </c>
-      <c r="T115" s="4">
-        <f t="shared" si="87"/>
-        <v>1.6014846455563876</v>
-      </c>
-      <c r="U115" s="4">
-        <f t="shared" si="88"/>
-        <v>8.6421068204179665</v>
-      </c>
-      <c r="V115" s="5">
-        <f t="shared" si="89"/>
-        <v>43.210534102089831</v>
-      </c>
+      <c r="D115"/>
+      <c r="E115"/>
+      <c r="G115"/>
+      <c r="J115" s="2"/>
+      <c r="S115" s="4"/>
+      <c r="T115" s="4"/>
+      <c r="U115" s="4"/>
+      <c r="V115" s="5"/>
       <c r="W115" s="4"/>
-      <c r="X115" s="4">
-        <f t="shared" si="90"/>
-        <v>112.53426034246239</v>
-      </c>
-      <c r="Y115" s="4">
-        <f t="shared" si="91"/>
-        <v>562.6713017123119</v>
-      </c>
+      <c r="X115" s="4"/>
+      <c r="Y115" s="4"/>
     </row>
     <row r="116" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B116">
-        <v>8</v>
-      </c>
-      <c r="C116">
-        <v>35</v>
+      <c r="C116" t="s">
+        <v>375</v>
       </c>
       <c r="D116">
-        <v>2646.43226937078</v>
+        <v>2756.8</v>
       </c>
       <c r="E116">
-        <v>142.98892057288001</v>
+        <v>126.7</v>
       </c>
       <c r="F116">
-        <v>0.11490311377239</v>
+        <v>5.9945999999999999E-2</v>
       </c>
       <c r="G116">
-        <v>70.682741129194</v>
+        <v>35.43</v>
       </c>
       <c r="H116" s="1">
-        <f t="shared" si="78"/>
-        <v>62.355091317586549</v>
+        <f t="shared" ref="H115:H116" si="92">2*PI()*150000*Ipt*Ipt*D116*(10^-9)</f>
+        <v>64.955569705622565</v>
       </c>
       <c r="I116" s="1">
-        <f t="shared" si="79"/>
+        <f t="shared" ref="I115:I116" si="93">2*PI()*150000*Ist*Ist*E116*(10^-9)</f>
         <v>0</v>
       </c>
       <c r="J116" s="2">
-        <f t="shared" si="80"/>
+        <f t="shared" ref="J115:J116" si="94">F116*SQRT(H116*I116)</f>
         <v>0</v>
       </c>
       <c r="K116">
-        <f t="shared" si="81"/>
-        <v>0.33308457040059752</v>
+        <f t="shared" ref="K115:K116" si="95">2*PI()*150000*G116*Ipt*(10^-9)</f>
+        <v>0.16695994157502955</v>
       </c>
       <c r="N116">
-        <f t="shared" si="82"/>
-        <v>23.817890424337019</v>
+        <f t="shared" ref="N115:N116" si="96">D116*$D$1^2*10^-3</f>
+        <v>24.811199999999999</v>
       </c>
       <c r="O116">
-        <f t="shared" si="83"/>
-        <v>3.5747230143220001</v>
+        <f t="shared" ref="O115:O116" si="97">E116*$D$2^2*10^-3</f>
+        <v>3.1675</v>
       </c>
       <c r="P116">
-        <f t="shared" si="84"/>
-        <v>1.06024111693791</v>
+        <f t="shared" ref="P115:P116" si="98">G116*$D$1*$D$2*10^-3</f>
+        <v>0.53144999999999998</v>
       </c>
       <c r="Q116">
-        <f t="shared" si="85"/>
-        <v>0.11490311377239056</v>
+        <f t="shared" ref="Q115:Q116" si="99">P116/SQRT(N116*O116)</f>
+        <v>5.9948761435939635E-2</v>
       </c>
       <c r="S116" s="4">
-        <f t="shared" si="86"/>
-        <v>4.9962685560089621</v>
+        <f t="shared" ref="S115:S116" si="100">w*P116*10^-6*$G$1</f>
+        <v>2.504399123625443</v>
       </c>
       <c r="T116" s="4">
-        <f t="shared" si="87"/>
-        <v>1.4829696072815877</v>
+        <f t="shared" ref="T115:T116" si="101">P116*$G$1/O116</f>
+        <v>0.83891081294396208</v>
       </c>
       <c r="U116" s="4">
-        <f t="shared" si="88"/>
-        <v>7.4093144183779556</v>
+        <f t="shared" ref="U115:U116" si="102">S116*T116</f>
+        <v>2.1009675047367664</v>
       </c>
       <c r="V116" s="5">
-        <f t="shared" si="89"/>
-        <v>37.046572091889779</v>
+        <f t="shared" ref="V115:V116" si="103">U116*$N$1</f>
+        <v>10.504837523683833</v>
       </c>
       <c r="W116" s="4"/>
       <c r="X116" s="4">
-        <f t="shared" si="90"/>
-        <v>112.23916437165578</v>
+        <f t="shared" ref="X115:X116" si="104">w*N116*10^-6*$G$1</f>
+        <v>116.92002547012061</v>
       </c>
       <c r="Y116" s="4">
-        <f t="shared" si="91"/>
-        <v>561.19582185827892</v>
+        <f t="shared" ref="Y115:Y116" si="105">X116*$G$1</f>
+        <v>584.60012735060309</v>
       </c>
     </row>
     <row r="117" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B117">
-        <v>9</v>
-      </c>
-      <c r="C117">
+      <c r="D117"/>
+      <c r="E117"/>
+      <c r="G117"/>
+      <c r="J117" s="2"/>
+      <c r="S117" s="4"/>
+      <c r="T117" s="4"/>
+      <c r="U117" s="4"/>
+      <c r="V117" s="5"/>
+      <c r="W117" s="4"/>
+      <c r="X117" s="4"/>
+      <c r="Y117" s="4"/>
+    </row>
+    <row r="118" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="D118"/>
+      <c r="E118"/>
+      <c r="G118"/>
+      <c r="J118" s="2"/>
+      <c r="S118" s="4"/>
+      <c r="T118" s="4"/>
+      <c r="U118" s="4"/>
+      <c r="V118" s="5"/>
+      <c r="W118" s="4"/>
+      <c r="X118" s="4"/>
+      <c r="Y118" s="4"/>
+    </row>
+    <row r="119" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="D119"/>
+      <c r="E119"/>
+      <c r="G119"/>
+      <c r="J119" s="2"/>
+      <c r="S119" s="4"/>
+      <c r="T119" s="4"/>
+      <c r="U119" s="4"/>
+      <c r="V119" s="5"/>
+      <c r="W119" s="4"/>
+      <c r="X119" s="4"/>
+      <c r="Y119" s="4"/>
+    </row>
+    <row r="120" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="J120" s="2"/>
+      <c r="S120" s="4"/>
+      <c r="T120" s="4"/>
+      <c r="U120" s="4"/>
+      <c r="V120" s="5"/>
+      <c r="W120" s="4"/>
+      <c r="X120" s="4"/>
+      <c r="Y120" s="4"/>
+    </row>
+    <row r="121" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B121" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="J121" s="2"/>
+      <c r="S121" s="4"/>
+      <c r="T121" s="4"/>
+      <c r="U121" s="4"/>
+      <c r="V121" s="5"/>
+      <c r="W121" s="4"/>
+      <c r="X121" s="4"/>
+      <c r="Y121" s="4"/>
+    </row>
+    <row r="122" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B122" t="s">
+        <v>0</v>
+      </c>
+      <c r="C122" t="s">
+        <v>2</v>
+      </c>
+      <c r="D122" t="s">
+        <v>3</v>
+      </c>
+      <c r="E122" t="s">
+        <v>4</v>
+      </c>
+      <c r="F122" t="s">
+        <v>5</v>
+      </c>
+      <c r="G122" t="s">
+        <v>6</v>
+      </c>
+      <c r="J122" s="2"/>
+      <c r="S122" s="4"/>
+      <c r="T122" s="4"/>
+      <c r="U122" s="4"/>
+      <c r="V122" s="5"/>
+      <c r="W122" s="4"/>
+      <c r="X122" s="4"/>
+      <c r="Y122" s="4"/>
+    </row>
+    <row r="123" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B123">
+        <v>1</v>
+      </c>
+      <c r="C123">
+        <v>0</v>
+      </c>
+      <c r="D123">
+        <v>2004.58188300853</v>
+      </c>
+      <c r="E123">
+        <v>125.160729663577</v>
+      </c>
+      <c r="F123">
+        <v>8.7633391238179106E-2</v>
+      </c>
+      <c r="G123">
+        <v>43.895051410095498</v>
+      </c>
+      <c r="H123" s="1">
+        <f t="shared" ref="H123:H128" si="106">2*PI()*150000*Ipt*Ipt*D123*(10^-9)</f>
+        <v>47.231847878840938</v>
+      </c>
+      <c r="I123" s="1">
+        <f t="shared" ref="I123:I128" si="107">2*PI()*150000*Ist*Ist*E123*(10^-9)</f>
+        <v>0</v>
+      </c>
+      <c r="J123" s="2">
+        <f t="shared" ref="J123:J128" si="108">F123*SQRT(H123*I123)</f>
+        <v>0</v>
+      </c>
+      <c r="K123">
+        <f t="shared" ref="K123:K128" si="109">2*PI()*150000*G123*Ipt*(10^-9)</f>
+        <v>0.20685055655835347</v>
+      </c>
+      <c r="N123">
+        <f t="shared" ref="N123:N128" si="110">D123*$D$1^2*10^-3</f>
+        <v>18.041236947076769</v>
+      </c>
+      <c r="O123">
+        <f t="shared" ref="O123:O128" si="111">E123*$D$2^2*10^-3</f>
+        <v>3.1290182415894252</v>
+      </c>
+      <c r="P123">
+        <f t="shared" ref="P123:P128" si="112">G123*$D$1*$D$2*10^-3</f>
+        <v>0.65842577115143242</v>
+      </c>
+      <c r="Q123">
+        <f t="shared" ref="Q123:Q128" si="113">P123/SQRT(N123*O123)</f>
+        <v>8.7633391238179162E-2</v>
+      </c>
+      <c r="S123" s="4">
+        <f t="shared" ref="S123:S137" si="114">w*P123*10^-6*$G$1</f>
+        <v>3.1027583483753012</v>
+      </c>
+      <c r="T123" s="4">
+        <f t="shared" ref="T123:T137" si="115">P123*$G$1/O123</f>
+        <v>1.0521283679333497</v>
+      </c>
+      <c r="U123" s="4">
+        <f t="shared" ref="U123:U137" si="116">S123*T123</f>
+        <v>3.2645000771676815</v>
+      </c>
+      <c r="V123" s="5">
+        <f t="shared" ref="V123:V137" si="117">U123*$N$1</f>
+        <v>16.322500385838406</v>
+      </c>
+      <c r="W123" s="4"/>
+      <c r="X123" s="4">
+        <f t="shared" ref="X123:X137" si="118">w*N123*10^-6*$G$1</f>
+        <v>85.017326181913688</v>
+      </c>
+      <c r="Y123" s="4">
+        <f t="shared" ref="Y123:Y137" si="119">X123*$G$1</f>
+        <v>425.08663090956844</v>
+      </c>
+    </row>
+    <row r="124" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B124">
+        <v>2</v>
+      </c>
+      <c r="C124">
+        <v>10</v>
+      </c>
+      <c r="D124">
+        <v>2004.15513439756</v>
+      </c>
+      <c r="E124">
+        <v>125.14926912919699</v>
+      </c>
+      <c r="F124">
+        <v>8.5491982479351997E-2</v>
+      </c>
+      <c r="G124">
+        <v>42.815913538700201</v>
+      </c>
+      <c r="H124" s="1">
+        <f t="shared" si="106"/>
+        <v>47.221792851582293</v>
+      </c>
+      <c r="I124" s="1">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="J124" s="2">
+        <f t="shared" si="108"/>
+        <v>0</v>
+      </c>
+      <c r="K124">
+        <f t="shared" si="109"/>
+        <v>0.20176523914487449</v>
+      </c>
+      <c r="N124">
+        <f t="shared" si="110"/>
+        <v>18.037396209578041</v>
+      </c>
+      <c r="O124">
+        <f t="shared" si="111"/>
+        <v>3.128731728229925</v>
+      </c>
+      <c r="P124">
+        <f t="shared" si="112"/>
+        <v>0.64223870308050302</v>
+      </c>
+      <c r="Q124">
+        <f t="shared" si="113"/>
+        <v>8.5491982479352011E-2</v>
+      </c>
+      <c r="S124" s="4">
+        <f t="shared" si="114"/>
+        <v>3.0264785871731172</v>
+      </c>
+      <c r="T124" s="4">
+        <f t="shared" si="115"/>
+        <v>1.0263562984414911</v>
+      </c>
+      <c r="U124" s="4">
+        <f t="shared" si="116"/>
+        <v>3.1062453600434341</v>
+      </c>
+      <c r="V124" s="5">
+        <f t="shared" si="117"/>
+        <v>15.531226800217171</v>
+      </c>
+      <c r="W124" s="4"/>
+      <c r="X124" s="4">
+        <f t="shared" si="118"/>
+        <v>84.999227132848119</v>
+      </c>
+      <c r="Y124" s="4">
+        <f t="shared" si="119"/>
+        <v>424.99613566424057</v>
+      </c>
+    </row>
+    <row r="125" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B125">
+        <v>3</v>
+      </c>
+      <c r="C125">
+        <v>20</v>
+      </c>
+      <c r="D125">
+        <v>2004.0513396513099</v>
+      </c>
+      <c r="E125">
+        <v>125.210350748512</v>
+      </c>
+      <c r="F125">
+        <v>7.9653190901418702E-2</v>
+      </c>
+      <c r="G125">
+        <v>39.900442849549002</v>
+      </c>
+      <c r="H125" s="1">
+        <f t="shared" si="106"/>
+        <v>47.219347245490042</v>
+      </c>
+      <c r="I125" s="1">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="J125" s="2">
+        <f t="shared" si="108"/>
+        <v>0</v>
+      </c>
+      <c r="K125">
+        <f t="shared" si="109"/>
+        <v>0.18802640719668384</v>
+      </c>
+      <c r="N125">
+        <f t="shared" si="110"/>
+        <v>18.03646205686179</v>
+      </c>
+      <c r="O125">
+        <f t="shared" si="111"/>
+        <v>3.1302587687128001</v>
+      </c>
+      <c r="P125">
+        <f t="shared" si="112"/>
+        <v>0.59850664274323506</v>
+      </c>
+      <c r="Q125">
+        <f t="shared" si="113"/>
+        <v>7.9653190901418661E-2</v>
+      </c>
+      <c r="S125" s="4">
+        <f t="shared" si="114"/>
+        <v>2.8203961079502573</v>
+      </c>
+      <c r="T125" s="4">
+        <f t="shared" si="115"/>
+        <v>0.95600186272994325</v>
+      </c>
+      <c r="U125" s="4">
+        <f t="shared" si="116"/>
+        <v>2.6963039328367282</v>
+      </c>
+      <c r="V125" s="5">
+        <f t="shared" si="117"/>
+        <v>13.48151966418364</v>
+      </c>
+      <c r="W125" s="4"/>
+      <c r="X125" s="4">
+        <f t="shared" si="118"/>
+        <v>84.994825041882081</v>
+      </c>
+      <c r="Y125" s="4">
+        <f t="shared" si="119"/>
+        <v>424.97412520941043</v>
+      </c>
+    </row>
+    <row r="126" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B126">
+        <v>4</v>
+      </c>
+      <c r="C126">
+        <v>30</v>
+      </c>
+      <c r="D126">
+        <v>1998.21955825195</v>
+      </c>
+      <c r="E126">
+        <v>125.01835797647701</v>
+      </c>
+      <c r="F126">
+        <v>7.0339133871971798E-2</v>
+      </c>
+      <c r="G126">
+        <v>35.156490432944302</v>
+      </c>
+      <c r="H126" s="1">
+        <f t="shared" si="106"/>
+        <v>47.081939133478258</v>
+      </c>
+      <c r="I126" s="1">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="J126" s="2">
+        <f t="shared" si="108"/>
+        <v>0</v>
+      </c>
+      <c r="K126">
+        <f t="shared" si="109"/>
+        <v>0.16567105810520649</v>
+      </c>
+      <c r="N126">
+        <f t="shared" si="110"/>
+        <v>17.983976024267552</v>
+      </c>
+      <c r="O126">
+        <f t="shared" si="111"/>
+        <v>3.1254589494119251</v>
+      </c>
+      <c r="P126">
+        <f t="shared" si="112"/>
+        <v>0.52734735649416453</v>
+      </c>
+      <c r="Q126">
+        <f t="shared" si="113"/>
+        <v>7.0339133871971909E-2</v>
+      </c>
+      <c r="S126" s="4">
+        <f t="shared" si="114"/>
+        <v>2.4850658715780973</v>
+      </c>
+      <c r="T126" s="4">
+        <f t="shared" si="115"/>
+        <v>0.84363187139826024</v>
+      </c>
+      <c r="U126" s="4">
+        <f t="shared" si="116"/>
+        <v>2.096480771787379</v>
+      </c>
+      <c r="V126" s="5">
+        <f t="shared" si="117"/>
+        <v>10.482403858936895</v>
+      </c>
+      <c r="W126" s="4"/>
+      <c r="X126" s="4">
+        <f t="shared" si="118"/>
+        <v>84.747490440260862</v>
+      </c>
+      <c r="Y126" s="4">
+        <f t="shared" si="119"/>
+        <v>423.73745220130434</v>
+      </c>
+    </row>
+    <row r="127" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B127">
+        <v>5</v>
+      </c>
+      <c r="C127">
         <v>40</v>
       </c>
-      <c r="D117">
-        <v>2641.6062832468901</v>
-      </c>
-      <c r="E117">
-        <v>142.99337517183301</v>
-      </c>
-      <c r="F117">
-        <v>0.10512810601228199</v>
-      </c>
-      <c r="G117">
-        <v>64.611651706515801</v>
-      </c>
-      <c r="H117" s="1">
-        <f t="shared" si="78"/>
-        <v>62.241381698438012</v>
-      </c>
-      <c r="I117" s="1">
-        <f t="shared" si="79"/>
-        <v>0</v>
-      </c>
-      <c r="J117" s="2">
-        <f t="shared" si="80"/>
-        <v>0</v>
-      </c>
-      <c r="K117">
-        <f t="shared" si="81"/>
-        <v>0.30447523550623873</v>
-      </c>
-      <c r="N117">
-        <f t="shared" si="82"/>
-        <v>23.774456549222009</v>
-      </c>
-      <c r="O117">
-        <f t="shared" si="83"/>
-        <v>3.5748343792958255</v>
-      </c>
-      <c r="P117">
-        <f t="shared" si="84"/>
-        <v>0.96917477559773701</v>
-      </c>
-      <c r="Q117">
-        <f t="shared" si="85"/>
-        <v>0.10512810601228209</v>
-      </c>
-      <c r="S117" s="4">
-        <f t="shared" si="86"/>
-        <v>4.5671285325935802</v>
-      </c>
-      <c r="T117" s="4">
-        <f t="shared" si="87"/>
-        <v>1.3555519959342091</v>
-      </c>
-      <c r="U117" s="4">
-        <f t="shared" si="88"/>
-        <v>6.1909801980453034</v>
-      </c>
-      <c r="V117" s="5">
-        <f t="shared" si="89"/>
-        <v>30.954900990226516</v>
-      </c>
-      <c r="W117" s="4"/>
-      <c r="X117" s="4">
-        <f t="shared" si="90"/>
-        <v>112.03448705718841</v>
-      </c>
-      <c r="Y117" s="4">
-        <f t="shared" si="91"/>
-        <v>560.17243528594213</v>
-      </c>
-    </row>
-    <row r="118" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B118">
+      <c r="D127">
+        <v>1995.27945291629</v>
+      </c>
+      <c r="E127">
+        <v>124.870714772154</v>
+      </c>
+      <c r="F127">
+        <v>5.8308118158195602E-2</v>
+      </c>
+      <c r="G127">
+        <v>29.1045701268493</v>
+      </c>
+      <c r="H127" s="1">
+        <f t="shared" si="106"/>
+        <v>47.012664533553583</v>
+      </c>
+      <c r="I127" s="1">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="J127" s="2">
+        <f t="shared" si="108"/>
+        <v>0</v>
+      </c>
+      <c r="K127">
+        <f t="shared" si="109"/>
+        <v>0.13715205554459808</v>
+      </c>
+      <c r="N127">
+        <f t="shared" si="110"/>
+        <v>17.957515076246612</v>
+      </c>
+      <c r="O127">
+        <f t="shared" si="111"/>
+        <v>3.1217678693038504</v>
+      </c>
+      <c r="P127">
+        <f t="shared" si="112"/>
+        <v>0.43656855190273952</v>
+      </c>
+      <c r="Q127">
+        <f t="shared" si="113"/>
+        <v>5.8308118158195726E-2</v>
+      </c>
+      <c r="S127" s="4">
+        <f t="shared" si="114"/>
+        <v>2.0572808331689711</v>
+      </c>
+      <c r="T127" s="4">
+        <f t="shared" si="115"/>
+        <v>0.69923288690919494</v>
+      </c>
+      <c r="U127" s="4">
+        <f t="shared" si="116"/>
+        <v>1.4385184161596936</v>
+      </c>
+      <c r="V127" s="5">
+        <f t="shared" si="117"/>
+        <v>7.1925920807984678</v>
+      </c>
+      <c r="W127" s="4"/>
+      <c r="X127" s="4">
+        <f t="shared" si="118"/>
+        <v>84.622796160396462</v>
+      </c>
+      <c r="Y127" s="4">
+        <f t="shared" si="119"/>
+        <v>423.11398080198228</v>
+      </c>
+    </row>
+    <row r="128" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B128">
+        <v>6</v>
+      </c>
+      <c r="C128">
+        <v>50</v>
+      </c>
+      <c r="D128">
+        <v>1992.3721851356099</v>
+      </c>
+      <c r="E128">
+        <v>125.11930455139399</v>
+      </c>
+      <c r="F128">
+        <v>4.4324648866239102E-2</v>
+      </c>
+      <c r="G128">
+        <v>22.1305750922246</v>
+      </c>
+      <c r="H128" s="1">
+        <f t="shared" si="106"/>
+        <v>46.944163650290065</v>
+      </c>
+      <c r="I128" s="1">
+        <f t="shared" si="107"/>
+        <v>0</v>
+      </c>
+      <c r="J128" s="2">
+        <f t="shared" si="108"/>
+        <v>0</v>
+      </c>
+      <c r="K128">
+        <f t="shared" si="109"/>
+        <v>0.10428787819417508</v>
+      </c>
+      <c r="N128">
+        <f t="shared" si="110"/>
+        <v>17.931349666220488</v>
+      </c>
+      <c r="O128">
+        <f t="shared" si="111"/>
+        <v>3.1279826137848499</v>
+      </c>
+      <c r="P128">
+        <f t="shared" si="112"/>
+        <v>0.33195862638336898</v>
+      </c>
+      <c r="Q128">
+        <f t="shared" si="113"/>
+        <v>4.4324648866239172E-2</v>
+      </c>
+      <c r="S128" s="4">
+        <f t="shared" si="114"/>
+        <v>1.5643181729126261</v>
+      </c>
+      <c r="T128" s="4">
+        <f t="shared" si="115"/>
+        <v>0.53062735214774737</v>
+      </c>
+      <c r="U128" s="4">
+        <f t="shared" si="116"/>
+        <v>0.83007001000922875</v>
+      </c>
+      <c r="V128" s="5">
+        <f t="shared" si="117"/>
+        <v>4.1503500500461437</v>
+      </c>
+      <c r="W128" s="4"/>
+      <c r="X128" s="4">
+        <f t="shared" si="118"/>
+        <v>84.499494570522103</v>
+      </c>
+      <c r="Y128" s="4">
+        <f t="shared" si="119"/>
+        <v>422.49747285261049</v>
+      </c>
+    </row>
+    <row r="129" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="J129" s="2"/>
+      <c r="S129" s="4"/>
+      <c r="T129" s="4"/>
+      <c r="U129" s="4"/>
+      <c r="V129" s="5"/>
+      <c r="W129" s="4"/>
+      <c r="X129" s="4"/>
+      <c r="Y129" s="4"/>
+    </row>
+    <row r="130" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="J130" s="2"/>
+      <c r="S130" s="4"/>
+      <c r="T130" s="4"/>
+      <c r="U130" s="4"/>
+      <c r="V130" s="5"/>
+      <c r="W130" s="4"/>
+      <c r="X130" s="4"/>
+      <c r="Y130" s="4"/>
+    </row>
+    <row r="131" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B131" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="J131" s="2"/>
+      <c r="S131" s="4"/>
+      <c r="T131" s="4"/>
+      <c r="U131" s="4"/>
+      <c r="V131" s="5"/>
+      <c r="W131" s="4"/>
+      <c r="X131" s="4"/>
+      <c r="Y131" s="4"/>
+    </row>
+    <row r="132" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="C132">
+        <v>0</v>
+      </c>
+      <c r="D132">
+        <v>2039.8637443425</v>
+      </c>
+      <c r="E132">
+        <v>141.22991291272601</v>
+      </c>
+      <c r="F132">
+        <v>0.144636164448046</v>
+      </c>
+      <c r="G132">
+        <v>77.632008353281705</v>
+      </c>
+      <c r="H132" s="1">
+        <f t="shared" ref="H132:H137" si="120">2*PI()*150000*Ipt*Ipt*D132*(10^-9)</f>
+        <v>48.063157151629248</v>
+      </c>
+      <c r="I132" s="1">
+        <f t="shared" ref="I132:I137" si="121">2*PI()*150000*Ist*Ist*E132*(10^-9)</f>
+        <v>0</v>
+      </c>
+      <c r="J132" s="2">
+        <f t="shared" ref="J132:J137" si="122">F132*SQRT(H132*I132)</f>
+        <v>0</v>
+      </c>
+      <c r="K132">
+        <f t="shared" ref="K132:K137" si="123">2*PI()*150000*G132*Ipt*(10^-9)</f>
+        <v>0.36583222068913696</v>
+      </c>
+      <c r="N132">
+        <f t="shared" ref="N132:N137" si="124">D132*$D$1^2*10^-3</f>
+        <v>18.358773699082501</v>
+      </c>
+      <c r="O132">
+        <f t="shared" ref="O132:O137" si="125">E132*$D$2^2*10^-3</f>
+        <v>3.5307478228181504</v>
+      </c>
+      <c r="P132">
+        <f t="shared" ref="P132:P137" si="126">G132*$D$1*$D$2*10^-3</f>
+        <v>1.1644801252992256</v>
+      </c>
+      <c r="Q132">
+        <f t="shared" ref="Q132:Q137" si="127">P132/SQRT(N132*O132)</f>
+        <v>0.14463616444804603</v>
+      </c>
+      <c r="S132" s="4">
+        <f t="shared" si="114"/>
+        <v>5.4874833103370531</v>
+      </c>
+      <c r="T132" s="4">
+        <f t="shared" si="115"/>
+        <v>1.6490559277181229</v>
+      </c>
+      <c r="U132" s="4">
+        <f t="shared" si="116"/>
+        <v>9.0491668811655845</v>
+      </c>
+      <c r="V132" s="5">
+        <f t="shared" si="117"/>
+        <v>45.245834405827921</v>
+      </c>
+      <c r="W132" s="4"/>
+      <c r="X132" s="4">
+        <f t="shared" si="118"/>
+        <v>86.513682872932648</v>
+      </c>
+      <c r="Y132" s="4">
+        <f t="shared" si="119"/>
+        <v>432.56841436466323</v>
+      </c>
+    </row>
+    <row r="133" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="C133">
         <v>10</v>
       </c>
-      <c r="C118">
-        <v>45</v>
-      </c>
-      <c r="D118">
-        <v>2634.37520391521</v>
-      </c>
-      <c r="E118">
-        <v>142.65245691932299</v>
-      </c>
-      <c r="F118">
-        <v>9.3983947384347399E-2</v>
-      </c>
-      <c r="G118">
-        <v>57.614543431150103</v>
-      </c>
-      <c r="H118" s="1">
-        <f t="shared" si="78"/>
-        <v>62.07100340564353</v>
-      </c>
-      <c r="I118" s="1">
-        <f t="shared" si="79"/>
-        <v>0</v>
-      </c>
-      <c r="J118" s="2">
-        <f t="shared" si="80"/>
-        <v>0</v>
-      </c>
-      <c r="K118">
-        <f t="shared" si="81"/>
-        <v>0.27150213957484687</v>
-      </c>
-      <c r="N118">
-        <f t="shared" si="82"/>
-        <v>23.709376835236892</v>
-      </c>
-      <c r="O118">
-        <f t="shared" si="83"/>
-        <v>3.566311422983075</v>
-      </c>
-      <c r="P118">
-        <f t="shared" si="84"/>
-        <v>0.86421815146725156</v>
-      </c>
-      <c r="Q118">
-        <f t="shared" si="85"/>
-        <v>9.3983947384347399E-2</v>
-      </c>
-      <c r="S118" s="4">
-        <f t="shared" si="86"/>
-        <v>4.0725320936227032</v>
-      </c>
-      <c r="T118" s="4">
-        <f t="shared" si="87"/>
-        <v>1.2116414538250952</v>
-      </c>
-      <c r="U118" s="4">
-        <f t="shared" si="88"/>
-        <v>4.9344487066663714</v>
-      </c>
-      <c r="V118" s="5">
-        <f t="shared" si="89"/>
-        <v>24.672243533331859</v>
-      </c>
-      <c r="W118" s="4"/>
-      <c r="X118" s="4">
-        <f t="shared" si="90"/>
-        <v>111.72780613015834</v>
-      </c>
-      <c r="Y118" s="4">
-        <f t="shared" si="91"/>
-        <v>558.63903065079171</v>
-      </c>
-    </row>
-    <row r="119" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B119">
-        <v>11</v>
-      </c>
-      <c r="C119">
+      <c r="D133">
+        <v>2035.1747150291901</v>
+      </c>
+      <c r="E133">
+        <v>140.242441896256</v>
+      </c>
+      <c r="F133">
+        <v>0.139061412822157</v>
+      </c>
+      <c r="G133">
+        <v>74.2928842360689</v>
+      </c>
+      <c r="H133" s="1">
+        <f t="shared" si="120"/>
+        <v>47.952674501305538</v>
+      </c>
+      <c r="I133" s="1">
+        <f t="shared" si="121"/>
+        <v>0</v>
+      </c>
+      <c r="J133" s="2">
+        <f t="shared" si="122"/>
+        <v>0</v>
+      </c>
+      <c r="K133">
+        <f t="shared" si="123"/>
+        <v>0.35009696899504655</v>
+      </c>
+      <c r="N133">
+        <f t="shared" si="124"/>
+        <v>18.31657243526271</v>
+      </c>
+      <c r="O133">
+        <f t="shared" si="125"/>
+        <v>3.5060610474064</v>
+      </c>
+      <c r="P133">
+        <f t="shared" si="126"/>
+        <v>1.1143932635410334</v>
+      </c>
+      <c r="Q133">
+        <f t="shared" si="127"/>
+        <v>0.13906141282215698</v>
+      </c>
+      <c r="S133" s="4">
+        <f t="shared" si="114"/>
+        <v>5.2514545349256974</v>
+      </c>
+      <c r="T133" s="4">
+        <f t="shared" si="115"/>
+        <v>1.5892382483833289</v>
+      </c>
+      <c r="U133" s="4">
+        <f t="shared" si="116"/>
+        <v>8.3458124065500048</v>
+      </c>
+      <c r="V133" s="5">
+        <f t="shared" si="117"/>
+        <v>41.729062032750022</v>
+      </c>
+      <c r="W133" s="4"/>
+      <c r="X133" s="4">
+        <f t="shared" si="118"/>
+        <v>86.314814102349956</v>
+      </c>
+      <c r="Y133" s="4">
+        <f t="shared" si="119"/>
+        <v>431.57407051174977</v>
+      </c>
+    </row>
+    <row r="134" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="C134">
+        <v>20</v>
+      </c>
+      <c r="D134">
+        <v>2027.80941189179</v>
+      </c>
+      <c r="E134">
+        <v>138.25867448778999</v>
+      </c>
+      <c r="F134">
+        <v>0.123957503841301</v>
+      </c>
+      <c r="G134">
+        <v>65.634560859130801</v>
+      </c>
+      <c r="H134" s="1">
+        <f t="shared" si="120"/>
+        <v>47.77913363459615</v>
+      </c>
+      <c r="I134" s="1">
+        <f t="shared" si="121"/>
+        <v>0</v>
+      </c>
+      <c r="J134" s="2">
+        <f t="shared" si="122"/>
+        <v>0</v>
+      </c>
+      <c r="K134">
+        <f t="shared" si="123"/>
+        <v>0.30929558132495633</v>
+      </c>
+      <c r="N134">
+        <f t="shared" si="124"/>
+        <v>18.250284707026108</v>
+      </c>
+      <c r="O134">
+        <f t="shared" si="125"/>
+        <v>3.4564668621947501</v>
+      </c>
+      <c r="P134">
+        <f t="shared" si="126"/>
+        <v>0.98451841288696196</v>
+      </c>
+      <c r="Q134">
+        <f t="shared" si="127"/>
+        <v>0.12395750384130121</v>
+      </c>
+      <c r="S134" s="4">
+        <f t="shared" si="114"/>
+        <v>4.6394337198743427</v>
+      </c>
+      <c r="T134" s="4">
+        <f t="shared" si="115"/>
+        <v>1.424168742445028</v>
+      </c>
+      <c r="U134" s="4">
+        <f t="shared" si="116"/>
+        <v>6.6073364864905013</v>
+      </c>
+      <c r="V134" s="5">
+        <f t="shared" si="117"/>
+        <v>33.036682432452508</v>
+      </c>
+      <c r="W134" s="4"/>
+      <c r="X134" s="4">
+        <f t="shared" si="118"/>
+        <v>86.00244054227305</v>
+      </c>
+      <c r="Y134" s="4">
+        <f t="shared" si="119"/>
+        <v>430.01220271136526</v>
+      </c>
+    </row>
+    <row r="135" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="C135">
+        <v>30</v>
+      </c>
+      <c r="D135">
+        <v>2019.3894169964601</v>
+      </c>
+      <c r="E135">
+        <v>135.53102202236801</v>
+      </c>
+      <c r="F135">
+        <v>0.10154827757873799</v>
+      </c>
+      <c r="G135">
+        <v>53.125368569425497</v>
+      </c>
+      <c r="H135" s="1">
+        <f t="shared" si="120"/>
+        <v>47.580742178797905</v>
+      </c>
+      <c r="I135" s="1">
+        <f t="shared" si="121"/>
+        <v>0</v>
+      </c>
+      <c r="J135" s="2">
+        <f t="shared" si="122"/>
+        <v>0</v>
+      </c>
+      <c r="K135">
+        <f t="shared" si="123"/>
+        <v>0.25034740142543588</v>
+      </c>
+      <c r="N135">
+        <f t="shared" si="124"/>
+        <v>18.17450475296814</v>
+      </c>
+      <c r="O135">
+        <f t="shared" si="125"/>
+        <v>3.3882755505592006</v>
+      </c>
+      <c r="P135">
+        <f t="shared" si="126"/>
+        <v>0.79688052854138258</v>
+      </c>
+      <c r="Q135">
+        <f t="shared" si="127"/>
+        <v>0.10154827757873806</v>
+      </c>
+      <c r="S135" s="4">
+        <f t="shared" si="114"/>
+        <v>3.7552110213815384</v>
+      </c>
+      <c r="T135" s="4">
+        <f t="shared" si="115"/>
+        <v>1.1759381972488416</v>
+      </c>
+      <c r="U135" s="4">
+        <f t="shared" si="116"/>
+        <v>4.4158960787723878</v>
+      </c>
+      <c r="V135" s="5">
+        <f t="shared" si="117"/>
+        <v>22.079480393861939</v>
+      </c>
+      <c r="W135" s="4"/>
+      <c r="X135" s="4">
+        <f t="shared" si="118"/>
+        <v>85.645335921836235</v>
+      </c>
+      <c r="Y135" s="4">
+        <f t="shared" si="119"/>
+        <v>428.22667960918119</v>
+      </c>
+    </row>
+    <row r="136" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="C136">
+        <v>40</v>
+      </c>
+      <c r="D136">
+        <v>2007.52580203562</v>
+      </c>
+      <c r="E136">
+        <v>131.98080471728599</v>
+      </c>
+      <c r="F136">
+        <v>7.4131406077425202E-2</v>
+      </c>
+      <c r="G136">
+        <v>38.158227376831903</v>
+      </c>
+      <c r="H136" s="1">
+        <f t="shared" si="120"/>
+        <v>47.301212336752961</v>
+      </c>
+      <c r="I136" s="1">
+        <f t="shared" si="121"/>
+        <v>0</v>
+      </c>
+      <c r="J136" s="2">
+        <f t="shared" si="122"/>
+        <v>0</v>
+      </c>
+      <c r="K136">
+        <f t="shared" si="123"/>
+        <v>0.17981641020159603</v>
+      </c>
+      <c r="N136">
+        <f t="shared" si="124"/>
+        <v>18.067732218320579</v>
+      </c>
+      <c r="O136">
+        <f t="shared" si="125"/>
+        <v>3.2995201179321501</v>
+      </c>
+      <c r="P136">
+        <f t="shared" si="126"/>
+        <v>0.5723734106524786</v>
+      </c>
+      <c r="Q136">
+        <f t="shared" si="127"/>
+        <v>7.4131406077425271E-2</v>
+      </c>
+      <c r="S136" s="4">
+        <f t="shared" si="114"/>
+        <v>2.6972461530239404</v>
+      </c>
+      <c r="T136" s="4">
+        <f t="shared" si="115"/>
+        <v>0.86735857063237431</v>
+      </c>
+      <c r="U136" s="4">
+        <f t="shared" si="116"/>
+        <v>2.3394795679305154</v>
+      </c>
+      <c r="V136" s="5">
+        <f t="shared" si="117"/>
+        <v>11.697397839652577</v>
+      </c>
+      <c r="W136" s="4"/>
+      <c r="X136" s="4">
+        <f t="shared" si="118"/>
+        <v>85.142182206155326</v>
+      </c>
+      <c r="Y136" s="4">
+        <f t="shared" si="119"/>
+        <v>425.71091103077663</v>
+      </c>
+    </row>
+    <row r="137" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="C137">
         <v>50</v>
       </c>
-      <c r="D119">
-        <v>2629.1421678853499</v>
-      </c>
-      <c r="E119">
-        <v>142.631411297819</v>
-      </c>
-      <c r="F119">
-        <v>8.2286375099905801E-2</v>
-      </c>
-      <c r="G119">
-        <v>50.3897908992368</v>
-      </c>
-      <c r="H119" s="1">
-        <f t="shared" si="78"/>
-        <v>61.947702899038184</v>
-      </c>
-      <c r="I119" s="1">
-        <f t="shared" si="79"/>
-        <v>0</v>
-      </c>
-      <c r="J119" s="2">
-        <f t="shared" si="80"/>
-        <v>0</v>
-      </c>
-      <c r="K119">
-        <f t="shared" si="81"/>
-        <v>0.23745629535745222</v>
-      </c>
-      <c r="N119">
-        <f t="shared" si="82"/>
-        <v>23.662279510968151</v>
-      </c>
-      <c r="O119">
-        <f t="shared" si="83"/>
-        <v>3.565785282445475</v>
-      </c>
-      <c r="P119">
-        <f t="shared" si="84"/>
-        <v>0.75584686348855201</v>
-      </c>
-      <c r="Q119">
-        <f t="shared" si="85"/>
-        <v>8.2286375099905718E-2</v>
-      </c>
-      <c r="S119" s="4">
-        <f t="shared" si="86"/>
-        <v>3.5618444303617833</v>
-      </c>
-      <c r="T119" s="4">
-        <f t="shared" si="87"/>
-        <v>1.0598603163370786</v>
-      </c>
-      <c r="U119" s="4">
-        <f t="shared" si="88"/>
-        <v>3.7750575647067008</v>
-      </c>
-      <c r="V119" s="5">
-        <f t="shared" si="89"/>
-        <v>18.875287823533505</v>
-      </c>
-      <c r="W119" s="4"/>
-      <c r="X119" s="4">
-        <f t="shared" si="90"/>
-        <v>111.50586521826874</v>
-      </c>
-      <c r="Y119" s="4">
-        <f t="shared" si="91"/>
-        <v>557.52932609134371</v>
+      <c r="D137">
+        <v>1999.06498930416</v>
+      </c>
+      <c r="E137">
+        <v>128.99100524109599</v>
+      </c>
+      <c r="F137">
+        <v>4.4685689702723103E-2</v>
+      </c>
+      <c r="G137">
+        <v>22.6914179811913</v>
+      </c>
+      <c r="H137" s="1">
+        <f t="shared" si="120"/>
+        <v>47.10185913334881</v>
+      </c>
+      <c r="I137" s="1">
+        <f t="shared" si="121"/>
+        <v>0</v>
+      </c>
+      <c r="J137" s="2">
+        <f t="shared" si="122"/>
+        <v>0</v>
+      </c>
+      <c r="K137">
+        <f t="shared" si="123"/>
+        <v>0.10693078804386888</v>
+      </c>
+      <c r="N137">
+        <f t="shared" si="124"/>
+        <v>17.99158490373744</v>
+      </c>
+      <c r="O137">
+        <f t="shared" si="125"/>
+        <v>3.2247751310273998</v>
+      </c>
+      <c r="P137">
+        <f t="shared" si="126"/>
+        <v>0.34037126971786952</v>
+      </c>
+      <c r="Q137">
+        <f t="shared" si="127"/>
+        <v>4.4685689702722999E-2</v>
+      </c>
+      <c r="S137" s="4">
+        <f t="shared" si="114"/>
+        <v>1.6039618206580331</v>
+      </c>
+      <c r="T137" s="4">
+        <f t="shared" si="115"/>
+        <v>0.52774419283218155</v>
+      </c>
+      <c r="U137" s="4">
+        <f t="shared" si="116"/>
+        <v>0.84648153637681001</v>
+      </c>
+      <c r="V137" s="5">
+        <f t="shared" si="117"/>
+        <v>4.2324076818840499</v>
+      </c>
+      <c r="W137" s="4"/>
+      <c r="X137" s="4">
+        <f t="shared" si="118"/>
+        <v>84.783346440027842</v>
+      </c>
+      <c r="Y137" s="4">
+        <f t="shared" si="119"/>
+        <v>423.91673220013922</v>
       </c>
     </row>
   </sheetData>
@@ -14404,7 +15116,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09A4C672-24E7-44AA-9133-057EC6FAFF93}">
   <dimension ref="B1:AA123"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
+    <sheetView topLeftCell="F86" workbookViewId="0">
       <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
@@ -24947,8 +25659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C17C92A-511E-405A-AC65-947739AFAEE7}">
   <dimension ref="B34"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="N35" sqref="N35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>